<commit_message>
Correcion matriz y correcion de feature
</commit_message>
<xml_diff>
--- a/Correction/Matriz de Riesgos Amazon.xlsx
+++ b/Correction/Matriz de Riesgos Amazon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josro\OneDrive\Documentos\JORGE\SOFKA\TrainingQA\T2-2\2024-C1-QA-FP-T02\Correction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5484B0B4-077F-4F9D-955D-91EB7E70D2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54467CEF-3016-49D8-8B14-67D5F6F6A714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A800537-A2B4-4BC5-85E7-4764F8D1D713}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
   <si>
     <t>Amazon, sistemas de login y registro</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Sugerir</t>
   </si>
   <si>
-    <t>Perdida de informacion por la actualizacion de la nueva base de datos</t>
-  </si>
-  <si>
     <t>Restraso del proyecto por falta de recursos financieros.</t>
   </si>
   <si>
@@ -318,18 +315,9 @@
     <t>Buscar un desarrollador Frontend que pueda cubrir su incapacidad.</t>
   </si>
   <si>
-    <t>Contactar al proveedor sobre los terminosndel contrato e intentar conseguir un acuerdo o nuevo proveedor.</t>
-  </si>
-  <si>
     <t>Backend developers</t>
   </si>
   <si>
-    <t>Atraso de produccion en entorno de desarrollo frontend debido a ausencia repentina de un desarrollador fronted por  enfermedad repentina.</t>
-  </si>
-  <si>
-    <t>Pérdida de servicios debidó a cambio de políticas del proveedor o tercero</t>
-  </si>
-  <si>
     <t>Hacer pruebas exhaustivas en el modulo de login</t>
   </si>
   <si>
@@ -345,9 +333,6 @@
     <t>Hacer pruebas exhaustivas en el modulo de cambio de datos y corregir errores</t>
   </si>
   <si>
-    <t>Transacciones incompletas debido a un mal diseño en el modulo de confirmar.</t>
-  </si>
-  <si>
     <t>Hacer pruebas exhaustivas del modulo de compras para asegurar su funcionamiento correcto.</t>
   </si>
   <si>
@@ -364,13 +349,34 @@
   </si>
   <si>
     <t>Francisco-Julio</t>
+  </si>
+  <si>
+    <t>Perdida de informacion de clientes por migracion de la base de datos a un nuevo servidor</t>
+  </si>
+  <si>
+    <t>Atraso de produccion en entorno de desarrollo frontend debido a ausencia inesperada de un desarrollador por  enfermedad repentina.</t>
+  </si>
+  <si>
+    <t>Pérdida de servicios de infraestrutura de redes debidó a cambio de políticas del proveedor o tercero</t>
+  </si>
+  <si>
+    <t>Contactar al proveedor sobre los terminos del contrato e intentar conseguir un acuerdo o nuevo proveedor.</t>
+  </si>
+  <si>
+    <t>Transacciones incompletas debido a un mal diseño UI en el modulo de confirmar.</t>
+  </si>
+  <si>
+    <t>Backend frontend</t>
+  </si>
+  <si>
+    <t>Equipo de desarrollo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,30 +411,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4472C4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -455,8 +437,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,12 +471,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -543,14 +524,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -735,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -756,12 +731,170 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -774,224 +907,64 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1336,7 +1309,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,9 +1360,9 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="90"/>
+        <v>100</v>
+      </c>
+      <c r="D3" s="29"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -1405,9 +1378,9 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="90"/>
+        <v>101</v>
+      </c>
+      <c r="D4" s="29"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -1419,13 +1392,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="90"/>
+        <v>103</v>
+      </c>
+      <c r="D5" s="29"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1437,13 +1410,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="91"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1461,427 +1434,427 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="92"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="95" t="s">
+      <c r="E8" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="95" t="s">
+      <c r="G8" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="95" t="s">
+      <c r="I8" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="K8" s="95" t="s">
+      <c r="K8" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="L8" s="95" t="s">
+      <c r="L8" s="32" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="97">
+      <c r="A9" s="34">
         <v>1</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="38">
+        <v>5</v>
+      </c>
+      <c r="E9" s="34">
+        <v>5</v>
+      </c>
+      <c r="F9" s="34">
+        <v>1</v>
+      </c>
+      <c r="G9" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L9" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>2</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="34">
+        <v>5</v>
+      </c>
+      <c r="E10" s="34">
+        <v>1</v>
+      </c>
+      <c r="F10" s="34">
+        <v>5</v>
+      </c>
+      <c r="G10" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L10" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
+        <v>3</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="34">
+        <v>5</v>
+      </c>
+      <c r="E11" s="34">
+        <v>1</v>
+      </c>
+      <c r="F11" s="34">
+        <v>5</v>
+      </c>
+      <c r="G11" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L11" s="37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
+        <v>4</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="34">
+        <v>5</v>
+      </c>
+      <c r="E12" s="34">
+        <v>1</v>
+      </c>
+      <c r="F12" s="34">
+        <v>4</v>
+      </c>
+      <c r="G12" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="K12" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L12" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>5</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="97">
+      <c r="C13" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="34">
         <v>5</v>
       </c>
-      <c r="E9" s="97">
+      <c r="E13" s="34">
         <v>5</v>
       </c>
-      <c r="F9" s="97">
+      <c r="F13" s="34">
         <v>2</v>
       </c>
-      <c r="G9" s="102" t="s">
+      <c r="G13" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="98" t="s">
+      <c r="H13" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="96" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="97" t="s">
+      <c r="I13" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="K9" s="99">
+      <c r="J13" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="36">
         <v>45363</v>
       </c>
-      <c r="L9" s="100" t="s">
+      <c r="L13" s="37" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="97">
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>6</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="34">
+        <v>5</v>
+      </c>
+      <c r="E14" s="34">
+        <v>1</v>
+      </c>
+      <c r="F14" s="34">
+        <v>5</v>
+      </c>
+      <c r="G14" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
+        <v>7</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="34">
+        <v>5</v>
+      </c>
+      <c r="E15" s="34">
         <v>2</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="F15" s="34">
+        <v>4</v>
+      </c>
+      <c r="G15" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L15" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="34">
         <v>8</v>
       </c>
-      <c r="C10" s="96" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="105">
+      <c r="B16" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="34">
         <v>5</v>
       </c>
-      <c r="E10" s="97">
+      <c r="E16" s="34">
+        <v>2</v>
+      </c>
+      <c r="F16" s="34">
+        <v>3</v>
+      </c>
+      <c r="G16" s="100" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L16" s="37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="34">
+        <v>9</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="97">
-        <v>1</v>
-      </c>
-      <c r="G10" s="103" t="s">
+      <c r="E17" s="34">
+        <v>3</v>
+      </c>
+      <c r="F17" s="34">
+        <v>5</v>
+      </c>
+      <c r="G17" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="36">
+        <v>45363</v>
+      </c>
+      <c r="L17" s="37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="34">
         <v>10</v>
       </c>
-      <c r="H10" s="98" t="s">
+      <c r="B18" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="34">
+        <v>5</v>
+      </c>
+      <c r="E18" s="34">
+        <v>3</v>
+      </c>
+      <c r="F18" s="34">
+        <v>4</v>
+      </c>
+      <c r="G18" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="96" t="s">
-        <v>87</v>
-      </c>
-      <c r="J10" s="97" t="s">
-        <v>88</v>
-      </c>
-      <c r="K10" s="99">
+      <c r="I18" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="36">
         <v>45363</v>
       </c>
-      <c r="L10" s="100" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="97">
-        <v>3</v>
-      </c>
-      <c r="B11" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="96" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="97">
-        <v>5</v>
-      </c>
-      <c r="E11" s="97">
-        <v>1</v>
-      </c>
-      <c r="F11" s="97">
-        <v>2</v>
-      </c>
-      <c r="G11" s="104" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I11" s="96" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="97" t="s">
-        <v>88</v>
-      </c>
-      <c r="K11" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L11" s="100" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="97">
-        <v>4</v>
-      </c>
-      <c r="B12" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="96" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="97">
-        <v>5</v>
-      </c>
-      <c r="E12" s="97">
-        <v>4</v>
-      </c>
-      <c r="F12" s="97">
-        <v>2</v>
-      </c>
-      <c r="G12" s="102" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I12" s="96" t="s">
-        <v>92</v>
-      </c>
-      <c r="J12" s="97" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L12" s="100" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="97">
-        <v>5</v>
-      </c>
-      <c r="B13" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="96" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="97">
-        <v>5</v>
-      </c>
-      <c r="E13" s="97">
-        <v>1</v>
-      </c>
-      <c r="F13" s="97">
-        <v>4</v>
-      </c>
-      <c r="G13" s="104" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" s="96" t="s">
-        <v>93</v>
-      </c>
-      <c r="J13" s="97" t="s">
-        <v>88</v>
-      </c>
-      <c r="K13" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L13" s="100" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="97">
-        <v>6</v>
-      </c>
-      <c r="B14" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="97">
-        <v>5</v>
-      </c>
-      <c r="E14" s="97">
-        <v>1</v>
-      </c>
-      <c r="F14" s="97">
-        <v>5</v>
-      </c>
-      <c r="G14" s="103" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="96" t="s">
-        <v>101</v>
-      </c>
-      <c r="J14" s="96" t="s">
-        <v>94</v>
-      </c>
-      <c r="K14" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L14" s="100" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="97">
-        <v>7</v>
-      </c>
-      <c r="B15" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="96" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="97">
-        <v>5</v>
-      </c>
-      <c r="E15" s="97">
-        <v>2</v>
-      </c>
-      <c r="F15" s="97">
-        <v>4</v>
-      </c>
-      <c r="G15" s="102" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I15" s="96" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="K15" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L15" s="100" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="97">
-        <v>8</v>
-      </c>
-      <c r="B16" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="97">
-        <v>5</v>
-      </c>
-      <c r="E16" s="97">
-        <v>2</v>
-      </c>
-      <c r="F16" s="97">
-        <v>3</v>
-      </c>
-      <c r="G16" s="103" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" s="96" t="s">
-        <v>103</v>
-      </c>
-      <c r="J16" s="96" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L16" s="100" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="97">
-        <v>9</v>
-      </c>
-      <c r="B17" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="96" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" s="97">
-        <v>5</v>
-      </c>
-      <c r="E17" s="97">
-        <v>3</v>
-      </c>
-      <c r="F17" s="97">
-        <v>5</v>
-      </c>
-      <c r="G17" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I17" s="96" t="s">
-        <v>97</v>
-      </c>
-      <c r="J17" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="K17" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L17" s="100" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="97">
-        <v>10</v>
-      </c>
-      <c r="B18" s="97" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="96" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="97">
-        <v>5</v>
-      </c>
-      <c r="E18" s="97">
-        <v>3</v>
-      </c>
-      <c r="F18" s="97">
-        <v>4</v>
-      </c>
-      <c r="G18" s="101" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I18" s="96" t="s">
-        <v>99</v>
-      </c>
-      <c r="J18" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="K18" s="99">
-        <v>45363</v>
-      </c>
-      <c r="L18" s="100" t="s">
+      <c r="L18" s="37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2105,7 +2078,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T25" sqref="S25:T25"/>
+      <selection activeCell="G22" sqref="G22:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,14 +2169,14 @@
       <c r="Q4" s="15"/>
     </row>
     <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="81"/>
+      <c r="C5" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="81"/>
       <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
@@ -2223,15 +2196,15 @@
       <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="24" t="s">
+      <c r="B6" s="83"/>
+      <c r="C6" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="89">
+      <c r="D6" s="83"/>
+      <c r="E6" s="28">
         <v>45365</v>
       </c>
       <c r="F6" s="5"/>
@@ -2271,22 +2244,22 @@
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="32" t="s">
+      <c r="B8" s="85"/>
+      <c r="C8" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="91"/>
+      <c r="L8" s="91"/>
       <c r="M8" s="5"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -2294,18 +2267,18 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
+      <c r="A9" s="86"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
       <c r="M9" s="5"/>
       <c r="N9" s="17" t="s">
         <v>29</v>
@@ -2315,28 +2288,28 @@
       <c r="Q9" s="15"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="36" t="s">
+      <c r="A10" s="86"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="36" t="s">
+      <c r="D10" s="94"/>
+      <c r="E10" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="36" t="s">
+      <c r="F10" s="94"/>
+      <c r="G10" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="40" t="s">
+      <c r="H10" s="94"/>
+      <c r="I10" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="J10" s="41"/>
-      <c r="K10" s="36" t="s">
+      <c r="J10" s="97"/>
+      <c r="K10" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="L10" s="44"/>
+      <c r="L10" s="75"/>
       <c r="M10" s="5"/>
       <c r="N10" s="14" t="s">
         <v>30</v>
@@ -2346,18 +2319,18 @@
       <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="45"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="95"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="77"/>
       <c r="M11" s="5"/>
       <c r="N11" s="14" t="s">
         <v>31</v>
@@ -2367,32 +2340,32 @@
       <c r="Q11" s="15"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="45" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="52"/>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="58"/>
-      <c r="G12" s="63" t="s">
+      <c r="F12" s="62"/>
+      <c r="G12" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="63" t="s">
+      <c r="H12" s="66"/>
+      <c r="I12" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="64"/>
-      <c r="K12" s="63" t="s">
+      <c r="J12" s="66"/>
+      <c r="K12" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="69"/>
+      <c r="L12" s="71"/>
       <c r="M12" s="5"/>
       <c r="N12" s="14" t="s">
         <v>33</v>
@@ -2402,18 +2375,18 @@
       <c r="Q12" s="15"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="70"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="72"/>
       <c r="M13" s="5"/>
       <c r="N13" s="14" t="s">
         <v>34</v>
@@ -2423,18 +2396,18 @@
       <c r="Q13" s="15"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="70"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="72"/>
       <c r="M14" s="5"/>
       <c r="N14" s="19" t="s">
         <v>35</v>
@@ -2444,18 +2417,18 @@
       <c r="Q14" s="21"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="70"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="72"/>
       <c r="M15" s="5"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -2463,18 +2436,18 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="71"/>
+      <c r="A16" s="79"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="73"/>
       <c r="M16" s="5"/>
       <c r="N16" s="17" t="s">
         <v>36</v>
@@ -2484,122 +2457,122 @@
       <c r="Q16" s="15"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="48" t="s">
+      <c r="A17" s="79"/>
+      <c r="B17" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="45" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="52"/>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="45" t="s">
         <v>58</v>
       </c>
       <c r="F17" s="52"/>
-      <c r="G17" s="57" t="s">
+      <c r="G17" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="58"/>
-      <c r="I17" s="63" t="s">
+      <c r="H17" s="62"/>
+      <c r="I17" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="J17" s="64"/>
-      <c r="K17" s="63" t="s">
+      <c r="J17" s="66"/>
+      <c r="K17" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="L17" s="69"/>
+      <c r="L17" s="71"/>
       <c r="M17" s="5"/>
       <c r="N17" s="14" t="s">
         <v>37</v>
       </c>
       <c r="O17" s="18"/>
-      <c r="P17" s="83" t="s">
+      <c r="P17" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="Q17" s="88"/>
+      <c r="Q17" s="27"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="70"/>
+      <c r="A18" s="79"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="72"/>
       <c r="M18" s="5"/>
       <c r="N18" s="14" t="s">
         <v>38</v>
       </c>
       <c r="O18" s="18"/>
-      <c r="P18" s="83" t="s">
+      <c r="P18" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="Q18" s="87"/>
+      <c r="Q18" s="26"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="66"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="70"/>
+      <c r="A19" s="79"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="72"/>
       <c r="M19" s="5"/>
       <c r="N19" s="14" t="s">
         <v>39</v>
       </c>
       <c r="O19" s="18"/>
-      <c r="P19" s="83" t="s">
+      <c r="P19" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="Q19" s="86"/>
+      <c r="Q19" s="25"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="70"/>
+      <c r="A20" s="79"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="72"/>
       <c r="M20" s="5"/>
       <c r="N20" s="19" t="s">
         <v>40</v>
       </c>
       <c r="O20" s="20"/>
-      <c r="P20" s="84" t="s">
+      <c r="P20" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="Q20" s="85"/>
+      <c r="Q20" s="24"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="71"/>
+      <c r="A21" s="79"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="73"/>
       <c r="M21" s="5"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -2607,30 +2580,30 @@
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="48" t="s">
+      <c r="A22" s="79"/>
+      <c r="B22" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="51" t="s">
+      <c r="D22" s="42"/>
+      <c r="E22" s="45" t="s">
         <v>57</v>
       </c>
       <c r="F22" s="52"/>
-      <c r="G22" s="57" t="s">
+      <c r="G22" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="58"/>
-      <c r="I22" s="57" t="s">
+      <c r="H22" s="62"/>
+      <c r="I22" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="J22" s="58"/>
-      <c r="K22" s="63" t="s">
+      <c r="J22" s="62"/>
+      <c r="K22" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="69"/>
+      <c r="L22" s="71"/>
       <c r="M22" s="5"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -2638,18 +2611,18 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="70"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="72"/>
       <c r="M23" s="5"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -2657,18 +2630,18 @@
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="70"/>
+      <c r="A24" s="79"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="63"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="72"/>
       <c r="M24" s="5"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -2676,18 +2649,18 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="70"/>
+      <c r="A25" s="79"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="72"/>
       <c r="M25" s="5"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -2695,18 +2668,18 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="71"/>
+      <c r="A26" s="79"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="73"/>
       <c r="M26" s="5"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -2714,30 +2687,30 @@
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="48" t="s">
+      <c r="A27" s="79"/>
+      <c r="B27" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="73"/>
-      <c r="E27" s="72" t="s">
+      <c r="D27" s="42"/>
+      <c r="E27" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="73"/>
-      <c r="G27" s="51" t="s">
+      <c r="F27" s="42"/>
+      <c r="G27" s="45" t="s">
         <v>57</v>
       </c>
       <c r="H27" s="52"/>
-      <c r="I27" s="51" t="s">
+      <c r="I27" s="45" t="s">
         <v>59</v>
       </c>
       <c r="J27" s="52"/>
-      <c r="K27" s="57" t="s">
+      <c r="K27" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="L27" s="78"/>
+      <c r="L27" s="57"/>
       <c r="M27" s="5"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -2745,18 +2718,18 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="79"/>
+      <c r="A28" s="79"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="59"/>
       <c r="M28" s="5"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -2764,18 +2737,18 @@
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="79"/>
+      <c r="A29" s="79"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="59"/>
       <c r="M29" s="5"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -2783,18 +2756,18 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="79"/>
+      <c r="A30" s="79"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="59"/>
       <c r="M30" s="5"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -2802,18 +2775,18 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="80"/>
+      <c r="A31" s="79"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="61"/>
       <c r="M31" s="5"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2821,30 +2794,30 @@
       <c r="Q31" s="1"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="48" t="s">
+      <c r="A32" s="79"/>
+      <c r="B32" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="72" t="s">
+      <c r="C32" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="73"/>
-      <c r="E32" s="72" t="s">
+      <c r="D32" s="42"/>
+      <c r="E32" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="73"/>
-      <c r="G32" s="72" t="s">
+      <c r="F32" s="42"/>
+      <c r="G32" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="H32" s="73"/>
-      <c r="I32" s="72" t="s">
+      <c r="H32" s="42"/>
+      <c r="I32" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="J32" s="73"/>
-      <c r="K32" s="51" t="s">
+      <c r="J32" s="42"/>
+      <c r="K32" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="L32" s="81"/>
+      <c r="L32" s="46"/>
       <c r="M32" s="5"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -2852,18 +2825,18 @@
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="82"/>
+      <c r="A33" s="79"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="48"/>
       <c r="M33" s="5"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -2871,18 +2844,18 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="82"/>
+      <c r="A34" s="79"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="48"/>
       <c r="M34" s="5"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -2890,18 +2863,18 @@
       <c r="Q34" s="1"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="82"/>
+      <c r="A35" s="79"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="48"/>
       <c r="M35" s="5"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -2909,18 +2882,18 @@
       <c r="Q35" s="1"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="75"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="82"/>
+      <c r="A36" s="79"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="48"/>
       <c r="M36" s="5"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -2986,18 +2959,26 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:D36"/>
-    <mergeCell ref="E32:F36"/>
-    <mergeCell ref="G32:H36"/>
-    <mergeCell ref="I32:J36"/>
-    <mergeCell ref="K32:L36"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:D31"/>
-    <mergeCell ref="E27:F31"/>
-    <mergeCell ref="G27:H31"/>
-    <mergeCell ref="I27:J31"/>
-    <mergeCell ref="K27:L31"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A8:B11"/>
+    <mergeCell ref="C8:L9"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="A12:A36"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:D16"/>
+    <mergeCell ref="E12:F16"/>
+    <mergeCell ref="G12:H16"/>
+    <mergeCell ref="I12:J16"/>
+    <mergeCell ref="K12:L16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:D21"/>
     <mergeCell ref="E17:F21"/>
     <mergeCell ref="G17:H21"/>
     <mergeCell ref="I17:J21"/>
@@ -3008,26 +2989,18 @@
     <mergeCell ref="G22:H26"/>
     <mergeCell ref="I22:J26"/>
     <mergeCell ref="K22:L26"/>
-    <mergeCell ref="K10:L11"/>
-    <mergeCell ref="A12:A36"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:D16"/>
-    <mergeCell ref="E12:F16"/>
-    <mergeCell ref="G12:H16"/>
-    <mergeCell ref="I12:J16"/>
-    <mergeCell ref="K12:L16"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:D21"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A8:B11"/>
-    <mergeCell ref="C8:L9"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="K32:L36"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:D31"/>
+    <mergeCell ref="E27:F31"/>
+    <mergeCell ref="G27:H31"/>
+    <mergeCell ref="I27:J31"/>
+    <mergeCell ref="K27:L31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:D36"/>
+    <mergeCell ref="E32:F36"/>
+    <mergeCell ref="G32:H36"/>
+    <mergeCell ref="I32:J36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>